<commit_message>
WIP: heuristic solution work
</commit_message>
<xml_diff>
--- a/src/data/test_problems/3_comp_linear_hydrocarbons_test.xlsx
+++ b/src/data/test_problems/3_comp_linear_hydrocarbons_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Desktop\sns_modeling\src\data\test_problems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5993A673-CCC6-4FFB-A331-60817386BB41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB7DBA20-9707-45BE-BCF6-390C64885353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-2235" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="system" sheetId="1" r:id="rId1"/>
@@ -455,7 +455,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>